<commit_message>
#73 upload latest specs with controlled terminology
</commit_message>
<xml_diff>
--- a/metadata/ADSL_ADVS_spec.xlsx
+++ b/metadata/ADSL_ADVS_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanny.Gautier\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38911FAB-1D64-4B12-B5A8-126EF170450E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8401F15D-C7CF-4980-9BD1-A478FFE98BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28935" windowHeight="14670" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28935" windowHeight="14670" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Documents" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Codelists!$A$1:$H$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Codelists!$A$1:$H$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Comments!$A$1:$D$272</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Datasets!$A$1:$I$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Dictionaries!$A$1:$E$1</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="592">
   <si>
     <t>Attribute</t>
   </si>
@@ -1887,13 +1887,13 @@
 Set to 'Y' to the latest and highest value (ordering by Analysis Date [ADVS.ADT] and Analysis Value [ADVS.AVAL]) by USUBJID, PARAMCD, AVISIT,  ATPT, DTYPE.</t>
   </si>
   <si>
-    <t>ADSL.SAFFL</t>
-  </si>
-  <si>
     <t>SUPPDM.ITT</t>
   </si>
   <si>
     <t>SUPPDM.SAFETY</t>
+  </si>
+  <si>
+    <t>ADSL_AGEGR1</t>
   </si>
 </sst>
 </file>
@@ -2653,11 +2653,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M19" sqref="M19:M20"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3092,7 +3092,9 @@
       <c r="I11" t="s">
         <v>50</v>
       </c>
-      <c r="J11"/>
+      <c r="J11" t="s">
+        <v>591</v>
+      </c>
       <c r="K11" t="s">
         <v>85</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>50</v>
       </c>
       <c r="J15" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="K15" t="s">
         <v>268</v>
@@ -3286,7 +3288,7 @@
         <v>50</v>
       </c>
       <c r="J16" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="K16" t="s">
         <v>85</v>
@@ -3325,7 +3327,7 @@
         <v>50</v>
       </c>
       <c r="J17" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="K17" t="s">
         <v>268</v>
@@ -3404,13 +3406,13 @@
         <v>264</v>
       </c>
       <c r="K19" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="L19"/>
-      <c r="M19" t="s">
-        <v>386</v>
-      </c>
-      <c r="N19"/>
+      <c r="M19"/>
+      <c r="N19" s="12" t="s">
+        <v>589</v>
+      </c>
       <c r="O19" t="s">
         <v>283</v>
       </c>
@@ -3418,7 +3420,7 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>19</v>
       </c>
@@ -3445,11 +3447,12 @@
         <v>264</v>
       </c>
       <c r="K20" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="L20"/>
-      <c r="M20" t="s">
-        <v>589</v>
+      <c r="M20"/>
+      <c r="N20" s="12" t="s">
+        <v>590</v>
       </c>
       <c r="O20"/>
       <c r="P20"/>
@@ -7344,18 +7347,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="12" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="12" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="12" customWidth="1"/>
@@ -7396,20 +7399,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>262</v>
+        <v>591</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E2" s="22">
         <v>1</v>
       </c>
-      <c r="F2" s="22">
-        <v>1</v>
+      <c r="F2" s="20" t="s">
+        <v>464</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="20" t="s">
@@ -7418,20 +7421,20 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>262</v>
+        <v>591</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E3" s="22">
         <v>2</v>
       </c>
-      <c r="F3" s="22">
-        <v>2</v>
+      <c r="F3" s="20" t="s">
+        <v>465</v>
       </c>
       <c r="G3" s="21"/>
       <c r="H3" s="20" t="s">
@@ -7440,20 +7443,20 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>262</v>
+        <v>591</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E4" s="22">
         <v>3</v>
       </c>
-      <c r="F4" s="22">
-        <v>3</v>
+      <c r="F4" s="20" t="s">
+        <v>466</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="20" t="s">
@@ -7472,63 +7475,59 @@
         <v>226</v>
       </c>
       <c r="E5" s="22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5" s="22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="20" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B6" t="s">
-        <v>571</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
+      <c r="A6" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="21"/>
       <c r="D6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H6"/>
+        <v>226</v>
+      </c>
+      <c r="E6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="22">
+        <v>2</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="20" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B7" t="s">
-        <v>571</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
-      </c>
+      <c r="A7" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="21"/>
       <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7"/>
+        <v>226</v>
+      </c>
+      <c r="E7" s="22">
+        <v>3</v>
+      </c>
+      <c r="F7" s="22">
+        <v>3</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -7544,61 +7543,61 @@
         <v>84</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>468</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>469</v>
+        <v>105</v>
       </c>
       <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>572</v>
+        <v>263</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>571</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
         <v>84</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>572</v>
+        <v>263</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>571</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
         <v>84</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>99</v>
+        <v>468</v>
       </c>
       <c r="G10" t="s">
-        <v>109</v>
+        <v>469</v>
       </c>
       <c r="H10"/>
     </row>
@@ -7616,13 +7615,13 @@
         <v>84</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H11"/>
     </row>
@@ -7640,13 +7639,13 @@
         <v>84</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H12"/>
     </row>
@@ -7664,57 +7663,61 @@
         <v>84</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>470</v>
-      </c>
-      <c r="G13"/>
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>107</v>
+      </c>
       <c r="H13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C14"/>
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
       <c r="D14" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>211</v>
+        <v>84</v>
+      </c>
+      <c r="E14" s="23">
+        <v>4</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14" t="s">
-        <v>98</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
-      </c>
-      <c r="C15"/>
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
       <c r="D15" t="s">
-        <v>226</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>210</v>
+        <v>84</v>
+      </c>
+      <c r="E15" s="23">
+        <v>5</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>210</v>
+        <v>470</v>
       </c>
       <c r="G15"/>
-      <c r="H15" t="s">
-        <v>99</v>
-      </c>
+      <c r="H15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -7728,14 +7731,14 @@
         <v>226</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -7750,14 +7753,14 @@
         <v>226</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -7772,59 +7775,59 @@
         <v>226</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>470</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B19" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="23">
-        <v>1</v>
+        <v>226</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>214</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>471</v>
+        <v>214</v>
       </c>
       <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="3"/>
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B20" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="23">
-        <v>2</v>
+        <v>226</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>223</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>472</v>
+        <v>223</v>
       </c>
       <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="3"/>
+      <c r="H20" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -7838,10 +7841,10 @@
         <v>84</v>
       </c>
       <c r="E21" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
@@ -7850,51 +7853,47 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E22" s="23">
-        <v>1</v>
-      </c>
-      <c r="F22" s="23">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>472</v>
       </c>
       <c r="G22"/>
-      <c r="H22" t="s">
-        <v>471</v>
-      </c>
-      <c r="I22" s="17"/>
+      <c r="H22"/>
+      <c r="I22" s="16"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C23"/>
       <c r="D23" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E23" s="23">
-        <v>2</v>
-      </c>
-      <c r="F23" s="23">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>467</v>
       </c>
       <c r="G23"/>
-      <c r="H23" t="s">
-        <v>472</v>
-      </c>
+      <c r="H23"/>
       <c r="I23" s="16"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -7908,61 +7907,65 @@
         <v>226</v>
       </c>
       <c r="E24" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G24"/>
       <c r="H24" t="s">
-        <v>467</v>
-      </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="4"/>
+        <v>471</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>259</v>
+        <v>575</v>
       </c>
       <c r="B25" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="E25" s="23">
-        <v>1</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>473</v>
+        <v>2</v>
+      </c>
+      <c r="F25" s="23">
+        <v>2</v>
       </c>
       <c r="G25"/>
-      <c r="H25"/>
+      <c r="H25" t="s">
+        <v>472</v>
+      </c>
       <c r="I25" s="16"/>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>259</v>
+        <v>575</v>
       </c>
       <c r="B26" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="E26" s="23">
-        <v>2</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>474</v>
+        <v>3</v>
+      </c>
+      <c r="F26" s="23">
+        <v>3</v>
       </c>
       <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="3"/>
+      <c r="H26" t="s">
+        <v>467</v>
+      </c>
+      <c r="I26" s="16"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -7976,57 +7979,57 @@
         <v>84</v>
       </c>
       <c r="E27" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E28" s="23">
-        <v>1</v>
-      </c>
-      <c r="F28" s="23">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>474</v>
       </c>
       <c r="G28"/>
-      <c r="H28" s="23" t="s">
-        <v>473</v>
-      </c>
+      <c r="H28"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E29" s="23">
-        <v>2</v>
-      </c>
-      <c r="F29" s="23">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>467</v>
       </c>
       <c r="G29"/>
-      <c r="H29" s="23" t="s">
-        <v>474</v>
-      </c>
+      <c r="H29"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -8040,66 +8043,58 @@
         <v>226</v>
       </c>
       <c r="E30" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F30" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30"/>
       <c r="H30" s="23" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>576</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="C31"/>
       <c r="D31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" t="s">
-        <v>110</v>
-      </c>
-      <c r="H31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="E31" s="23">
+        <v>2</v>
+      </c>
+      <c r="F31" s="23">
+        <v>2</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31" s="23" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>576</v>
+        <v>260</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="C32"/>
       <c r="D32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" t="s">
-        <v>111</v>
-      </c>
-      <c r="H32" t="s">
-        <v>116</v>
+        <v>226</v>
+      </c>
+      <c r="E32" s="23">
+        <v>3</v>
+      </c>
+      <c r="F32" s="23">
+        <v>3</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32" s="23" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -8116,19 +8111,19 @@
         <v>84</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>576</v>
       </c>
@@ -8142,57 +8137,69 @@
         <v>84</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>475</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
-        <v>476</v>
+        <v>111</v>
       </c>
       <c r="H34" t="s">
-        <v>477</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>265</v>
+        <v>576</v>
       </c>
       <c r="B35" t="s">
-        <v>577</v>
-      </c>
-      <c r="C35"/>
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
       <c r="D35" t="s">
         <v>84</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G35"/>
-      <c r="H35"/>
+        <v>102</v>
+      </c>
+      <c r="G35" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>576</v>
       </c>
       <c r="B36" t="s">
-        <v>577</v>
-      </c>
-      <c r="C36"/>
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
       <c r="D36" t="s">
         <v>84</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="G36"/>
-      <c r="H36"/>
+        <v>475</v>
+      </c>
+      <c r="G36" t="s">
+        <v>476</v>
+      </c>
+      <c r="H36" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -8205,11 +8212,11 @@
       <c r="D37" t="s">
         <v>84</v>
       </c>
-      <c r="E37" s="23">
-        <v>3</v>
+      <c r="E37" s="23" t="s">
+        <v>211</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G37"/>
       <c r="H37"/>
@@ -8226,57 +8233,53 @@
         <v>84</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>479</v>
+        <v>210</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>478</v>
+        <v>92</v>
       </c>
       <c r="G38"/>
       <c r="H38"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B39" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C39"/>
       <c r="D39" t="s">
-        <v>226</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>211</v>
+        <v>84</v>
+      </c>
+      <c r="E39" s="23">
+        <v>3</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="G39"/>
-      <c r="H39" s="23" t="s">
-        <v>90</v>
-      </c>
+      <c r="H39"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B40" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C40"/>
       <c r="D40" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>210</v>
+        <v>479</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>210</v>
+        <v>478</v>
       </c>
       <c r="G40"/>
-      <c r="H40" s="23" t="s">
-        <v>92</v>
-      </c>
+      <c r="H40"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -8290,14 +8293,14 @@
         <v>226</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>479</v>
-      </c>
-      <c r="F41" s="23">
-        <v>3</v>
+        <v>211</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>211</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -8312,66 +8315,58 @@
         <v>226</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>479</v>
+        <v>210</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>479</v>
+        <v>210</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="23" t="s">
-        <v>478</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>480</v>
+        <v>266</v>
       </c>
       <c r="B43" t="s">
-        <v>481</v>
-      </c>
-      <c r="C43" t="s">
-        <v>89</v>
-      </c>
+        <v>578</v>
+      </c>
+      <c r="C43"/>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G43" t="s">
-        <v>113</v>
-      </c>
-      <c r="H43" t="s">
-        <v>50</v>
+        <v>479</v>
+      </c>
+      <c r="F43" s="23">
+        <v>3</v>
+      </c>
+      <c r="G43"/>
+      <c r="H43" s="23" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>480</v>
+        <v>266</v>
       </c>
       <c r="B44" t="s">
-        <v>481</v>
-      </c>
-      <c r="C44" t="s">
-        <v>89</v>
-      </c>
+        <v>578</v>
+      </c>
+      <c r="C44"/>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>210</v>
+        <v>479</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>473</v>
-      </c>
-      <c r="G44" t="s">
-        <v>482</v>
-      </c>
-      <c r="H44" t="s">
-        <v>483</v>
+        <v>479</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44" s="23" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -8388,16 +8383,16 @@
         <v>84</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="G45" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H45" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -8414,24 +8409,24 @@
         <v>84</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>103</v>
+        <v>473</v>
       </c>
       <c r="G46" t="s">
-        <v>114</v>
+        <v>482</v>
       </c>
       <c r="H46" t="s">
-        <v>49</v>
+        <v>483</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>267</v>
+        <v>480</v>
       </c>
       <c r="B47" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C47" t="s">
         <v>89</v>
@@ -8440,29 +8435,33 @@
         <v>84</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47"/>
+        <v>102</v>
+      </c>
+      <c r="G47" t="s">
+        <v>112</v>
+      </c>
       <c r="H47" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>264</v>
+        <v>480</v>
       </c>
       <c r="B48" t="s">
-        <v>485</v>
-      </c>
-      <c r="C48"/>
+        <v>481</v>
+      </c>
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
       <c r="D48" t="s">
         <v>84</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F48" s="23" t="s">
         <v>103</v>
@@ -8476,38 +8475,36 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B49" t="s">
-        <v>485</v>
-      </c>
-      <c r="C49"/>
+        <v>484</v>
+      </c>
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
       <c r="D49" t="s">
         <v>84</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" t="s">
-        <v>113</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="G49"/>
       <c r="H49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>264</v>
       </c>
       <c r="B50" t="s">
-        <v>486</v>
-      </c>
-      <c r="C50" t="s">
-        <v>89</v>
-      </c>
+        <v>485</v>
+      </c>
+      <c r="C50"/>
       <c r="D50" t="s">
         <v>84</v>
       </c>
@@ -8517,60 +8514,58 @@
       <c r="F50" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="G50"/>
-      <c r="H50"/>
+      <c r="G50" t="s">
+        <v>114</v>
+      </c>
+      <c r="H50" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>371</v>
+        <v>264</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
-      </c>
-      <c r="C51" t="s">
-        <v>434</v>
-      </c>
+        <v>485</v>
+      </c>
+      <c r="C51"/>
       <c r="D51" t="s">
         <v>84</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>435</v>
+        <v>93</v>
       </c>
       <c r="G51" t="s">
-        <v>436</v>
-      </c>
-      <c r="H51" s="23" t="s">
-        <v>437</v>
+        <v>113</v>
+      </c>
+      <c r="H51" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>371</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>486</v>
       </c>
       <c r="C52" t="s">
-        <v>434</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
         <v>84</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>438</v>
-      </c>
-      <c r="G52" t="s">
-        <v>439</v>
-      </c>
-      <c r="H52" s="23" t="s">
-        <v>440</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="G52"/>
+      <c r="H52"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -8586,16 +8581,16 @@
         <v>84</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="G53" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H53" s="23" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -8612,16 +8607,16 @@
         <v>84</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="G54" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H54" s="23" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -8638,16 +8633,16 @@
         <v>84</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="G55" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -8664,16 +8659,16 @@
         <v>84</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="G56" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="H56" s="23" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -8690,16 +8685,16 @@
         <v>84</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>463</v>
+        <v>223</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G57" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="H57" s="23" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -8716,16 +8711,16 @@
         <v>84</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F58" s="23" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="G58" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="H58" s="23" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -8742,65 +8737,69 @@
         <v>84</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>212</v>
+        <v>463</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="G59" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="H59" s="23" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>462</v>
+        <v>434</v>
       </c>
       <c r="D60" t="s">
         <v>84</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="G60" t="s">
-        <v>436</v>
-      </c>
-      <c r="H60"/>
+        <v>457</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>462</v>
+        <v>434</v>
       </c>
       <c r="D61" t="s">
         <v>84</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>438</v>
+        <v>459</v>
       </c>
       <c r="G61" t="s">
-        <v>439</v>
-      </c>
-      <c r="H61"/>
+        <v>460</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -8816,13 +8815,13 @@
         <v>84</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="G62" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H62"/>
     </row>
@@ -8840,13 +8839,13 @@
         <v>84</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="G63" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="H63"/>
     </row>
@@ -8864,13 +8863,13 @@
         <v>84</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F64" s="23" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="G64" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="H64"/>
     </row>
@@ -8888,13 +8887,13 @@
         <v>84</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="G65" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="H65"/>
     </row>
@@ -8912,13 +8911,13 @@
         <v>84</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>463</v>
+        <v>223</v>
       </c>
       <c r="F66" s="23" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G66" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="H66"/>
     </row>
@@ -8936,13 +8935,13 @@
         <v>84</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F67" s="23" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="G67" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="H67"/>
     </row>
@@ -8960,59 +8959,63 @@
         <v>84</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>212</v>
+        <v>463</v>
       </c>
       <c r="F68" s="23" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="G68" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="H68"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B69" t="s">
-        <v>347</v>
-      </c>
-      <c r="C69"/>
+        <v>160</v>
+      </c>
+      <c r="C69" t="s">
+        <v>462</v>
+      </c>
       <c r="D69" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="G69"/>
-      <c r="H69" t="s">
-        <v>435</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="G69" t="s">
+        <v>457</v>
+      </c>
+      <c r="H69"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B70" t="s">
-        <v>347</v>
-      </c>
-      <c r="C70"/>
+        <v>160</v>
+      </c>
+      <c r="C70" t="s">
+        <v>462</v>
+      </c>
       <c r="D70" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="G70"/>
-      <c r="H70" t="s">
-        <v>438</v>
-      </c>
+        <v>459</v>
+      </c>
+      <c r="G70" t="s">
+        <v>460</v>
+      </c>
+      <c r="H70"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -9026,14 +9029,14 @@
         <v>226</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G71"/>
       <c r="H71" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -9048,14 +9051,14 @@
         <v>226</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G72"/>
       <c r="H72" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -9070,14 +9073,14 @@
         <v>226</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F73" s="23" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="G73"/>
       <c r="H73" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -9092,14 +9095,14 @@
         <v>226</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G74"/>
       <c r="H74" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -9114,14 +9117,14 @@
         <v>226</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>463</v>
+        <v>223</v>
       </c>
       <c r="F75" s="23" t="s">
-        <v>463</v>
+        <v>223</v>
       </c>
       <c r="G75"/>
       <c r="H75" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -9136,14 +9139,14 @@
         <v>226</v>
       </c>
       <c r="E76" s="23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F76" s="23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G76"/>
       <c r="H76" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -9158,35 +9161,62 @@
         <v>226</v>
       </c>
       <c r="E77" s="23" t="s">
-        <v>212</v>
+        <v>463</v>
       </c>
       <c r="F77" s="23" t="s">
-        <v>212</v>
+        <v>463</v>
       </c>
       <c r="G77"/>
       <c r="H77" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>372</v>
+      </c>
+      <c r="B78" t="s">
+        <v>347</v>
+      </c>
+      <c r="C78"/>
+      <c r="D78" t="s">
+        <v>226</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="F78" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="G78"/>
+      <c r="H78" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>372</v>
+      </c>
+      <c r="B79" t="s">
+        <v>347</v>
+      </c>
+      <c r="C79"/>
+      <c r="D79" t="s">
+        <v>226</v>
+      </c>
+      <c r="E79" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F79" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="G79"/>
+      <c r="H79" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-    </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="11"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -9194,22 +9224,149 @@
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
     </row>
-    <row r="81" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+    </row>
     <row r="97" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="98" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="99" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -9323,8 +9480,10 @@
     <row r="207" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="208" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="209" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:H82" xr:uid="{96482083-CDB9-4891-8BB3-78DEBC79034F}"/>
+  <autoFilter ref="A1:H84" xr:uid="{96482083-CDB9-4891-8BB3-78DEBC79034F}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9392,9 +9551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10261,34 +10420,10 @@
         <v>570</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>590</v>
-      </c>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I61"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
-        <v>589</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>589</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>591</v>
-      </c>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I62"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>